<commit_message>
Uploading regional data and changing Swiss data from in 1000 to actual numbers
</commit_message>
<xml_diff>
--- a/Asylstatistik_Schweiz_201012.xlsx
+++ b/Asylstatistik_Schweiz_201012.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EC89F4-E116-4D7D-8B98-DDFD3EF95AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75ACA698-6551-483C-B395-5C4F7D851EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="876" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH-Nati" sheetId="5" r:id="rId1"/>
@@ -1470,7 +1470,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P5" sqref="P5"/>
     </sheetView>
@@ -1637,49 +1637,49 @@
         <v>2010</v>
       </c>
       <c r="B4" s="30">
-        <v>25.341999999999999</v>
+        <v>25342</v>
       </c>
       <c r="C4" s="30">
-        <v>10.763999999999999</v>
+        <v>10764</v>
       </c>
       <c r="D4" s="30">
-        <v>14.577999999999999</v>
+        <v>14578</v>
       </c>
       <c r="E4" s="30">
-        <v>7.5179999999999998</v>
+        <v>7518</v>
       </c>
       <c r="F4" s="30">
-        <v>2.9870000000000001</v>
+        <v>2987</v>
       </c>
       <c r="G4" s="30">
-        <v>4.5309999999999997</v>
+        <v>4531</v>
       </c>
       <c r="H4" s="30">
-        <v>1.0029999999999999</v>
+        <v>1003</v>
       </c>
       <c r="I4" s="30">
-        <v>0.157</v>
+        <v>157</v>
       </c>
       <c r="J4" s="30">
-        <v>0.84599999999999997</v>
+        <v>846</v>
       </c>
       <c r="K4" s="30">
-        <v>6.5149999999999997</v>
+        <v>6515</v>
       </c>
       <c r="L4" s="30">
-        <v>2.83</v>
+        <v>2830</v>
       </c>
       <c r="M4" s="30">
-        <v>3.6850000000000001</v>
+        <v>3685</v>
       </c>
       <c r="N4" s="30">
-        <v>17.824000000000002</v>
+        <v>17824</v>
       </c>
       <c r="O4" s="30">
-        <v>7.7770000000000001</v>
+        <v>7777</v>
       </c>
       <c r="P4" s="30">
-        <v>10.047000000000001</v>
+        <v>10047</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -61022,7 +61022,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>

<commit_message>
End of data preparation
- data preparation regional data for germany
- data preparation regional data for Switzerland (no specific employment information on regional level for Switzerland)
- for each Bundesland and canton a table with the relevant data was created
</commit_message>
<xml_diff>
--- a/Asylstatistik_Schweiz_201012.xlsx
+++ b/Asylstatistik_Schweiz_201012.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75ACA698-6551-483C-B395-5C4F7D851EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FE9CB2-84C3-4E84-947A-3B87A80A1BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="876" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH-Nati" sheetId="5" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="190">
   <si>
     <t>Total anerkannte 
 Flüchtlinge mit Asyl</t>
@@ -669,6 +669,9 @@
   <si>
     <t>Aufteilung</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
@@ -892,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1127,6 +1130,18 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -33736,29 +33751,30 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" style="19" customWidth="1"/>
-    <col min="2" max="16" width="7.7265625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.54296875" style="2"/>
+    <col min="1" max="2" width="19.7265625" style="19" customWidth="1"/>
+    <col min="3" max="17" width="7.7265625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="B1" s="20"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" s="21" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" s="21" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>10</v>
       </c>
@@ -33777,108 +33793,114 @@
       <c r="N2" s="60"/>
       <c r="O2" s="60"/>
       <c r="P2" s="60"/>
-    </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q2" s="60"/>
+    </row>
+    <row r="3" spans="1:20" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="68"/>
+      <c r="B3" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="67" t="s">
+        <v>1</v>
+      </c>
       <c r="G3" s="68"/>
       <c r="H3" s="68"/>
       <c r="I3" s="68"/>
       <c r="J3" s="68"/>
       <c r="K3" s="68"/>
       <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="62"/>
-      <c r="P3" s="63"/>
-    </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="68"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="63"/>
+    </row>
+    <row r="4" spans="1:20" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="73" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="70" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="71"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="71"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="27"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="72"/>
       <c r="O4" s="27"/>
-      <c r="P4" s="28"/>
-    </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28"/>
+    </row>
+    <row r="5" spans="1:20" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="8.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="8.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -33893,1366 +33915,1446 @@
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
-    </row>
-    <row r="7" spans="1:19" s="13" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q6" s="24"/>
+    </row>
+    <row r="7" spans="1:20" s="13" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="81"/>
+      <c r="C7" s="11">
         <v>25342</v>
       </c>
-      <c r="C7" s="12">
+      <c r="D7" s="12">
         <v>10764</v>
       </c>
-      <c r="D7" s="12">
+      <c r="E7" s="12">
         <v>14578</v>
       </c>
-      <c r="E7" s="26">
+      <c r="F7" s="26">
         <v>7518</v>
       </c>
-      <c r="F7" s="12">
+      <c r="G7" s="12">
         <v>2987</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H7" s="12">
         <v>4531</v>
       </c>
-      <c r="H7" s="12">
+      <c r="I7" s="12">
         <v>1003</v>
       </c>
-      <c r="I7" s="12">
+      <c r="J7" s="12">
         <v>157</v>
       </c>
-      <c r="J7" s="12">
+      <c r="K7" s="12">
         <v>846</v>
       </c>
-      <c r="K7" s="12">
+      <c r="L7" s="12">
         <v>6515</v>
       </c>
-      <c r="L7" s="12">
+      <c r="M7" s="12">
         <v>2830</v>
       </c>
-      <c r="M7" s="12">
+      <c r="N7" s="12">
         <v>3685</v>
       </c>
-      <c r="N7" s="26">
+      <c r="O7" s="26">
         <v>17824</v>
       </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <v>7777</v>
       </c>
-      <c r="P7" s="12">
+      <c r="Q7" s="12">
         <v>10047</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="15">
         <v>1800</v>
       </c>
-      <c r="C8" s="16">
+      <c r="D8" s="16">
         <v>743</v>
       </c>
-      <c r="D8" s="16">
+      <c r="E8" s="16">
         <v>1057</v>
       </c>
-      <c r="E8" s="15">
+      <c r="F8" s="15">
         <v>620</v>
       </c>
-      <c r="F8" s="16">
+      <c r="G8" s="16">
         <v>245</v>
       </c>
-      <c r="G8" s="16">
+      <c r="H8" s="16">
         <v>375</v>
       </c>
-      <c r="H8" s="17">
+      <c r="I8" s="17">
         <v>63</v>
       </c>
-      <c r="I8" s="16">
+      <c r="J8" s="16">
         <v>7</v>
       </c>
-      <c r="J8" s="16">
+      <c r="K8" s="16">
         <v>56</v>
       </c>
-      <c r="K8" s="17">
+      <c r="L8" s="17">
         <v>557</v>
       </c>
-      <c r="L8" s="16">
+      <c r="M8" s="16">
         <v>238</v>
       </c>
-      <c r="M8" s="16">
+      <c r="N8" s="16">
         <v>319</v>
       </c>
-      <c r="N8" s="15">
+      <c r="O8" s="15">
         <v>1180</v>
       </c>
-      <c r="O8" s="16">
+      <c r="P8" s="16">
         <v>498</v>
       </c>
-      <c r="P8" s="16">
+      <c r="Q8" s="16">
         <v>682</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C9" s="15">
         <v>149</v>
       </c>
-      <c r="C9" s="17">
+      <c r="D9" s="17">
         <v>57</v>
       </c>
-      <c r="D9" s="17">
+      <c r="E9" s="17">
         <v>92</v>
       </c>
-      <c r="E9" s="15">
+      <c r="F9" s="15">
         <v>75</v>
       </c>
-      <c r="F9" s="17">
+      <c r="G9" s="17">
         <v>33</v>
       </c>
-      <c r="G9" s="17">
+      <c r="H9" s="17">
         <v>42</v>
       </c>
-      <c r="H9" s="17">
+      <c r="I9" s="17">
         <v>14</v>
       </c>
-      <c r="I9" s="17">
-        <v>2</v>
-      </c>
       <c r="J9" s="17">
+        <v>2</v>
+      </c>
+      <c r="K9" s="17">
         <v>12</v>
       </c>
-      <c r="K9" s="17">
+      <c r="L9" s="17">
         <v>61</v>
       </c>
-      <c r="L9" s="17">
+      <c r="M9" s="17">
         <v>31</v>
       </c>
-      <c r="M9" s="17">
+      <c r="N9" s="17">
         <v>30</v>
       </c>
-      <c r="N9" s="15">
+      <c r="O9" s="15">
         <v>74</v>
       </c>
-      <c r="O9" s="17">
+      <c r="P9" s="17">
         <v>24</v>
       </c>
-      <c r="P9" s="17">
+      <c r="Q9" s="17">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="15">
         <v>21</v>
       </c>
-      <c r="C10" s="16">
+      <c r="D10" s="16">
         <v>5</v>
       </c>
-      <c r="D10" s="16">
+      <c r="E10" s="16">
         <v>16</v>
       </c>
-      <c r="E10" s="15">
+      <c r="F10" s="15">
         <v>12</v>
       </c>
-      <c r="F10" s="16">
-        <v>2</v>
-      </c>
       <c r="G10" s="16">
+        <v>2</v>
+      </c>
+      <c r="H10" s="16">
         <v>10</v>
       </c>
-      <c r="H10" s="17">
+      <c r="I10" s="17">
         <v>7</v>
       </c>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
       <c r="J10" s="16">
+        <v>0</v>
+      </c>
+      <c r="K10" s="16">
         <v>7</v>
       </c>
-      <c r="K10" s="17">
+      <c r="L10" s="17">
         <v>5</v>
       </c>
-      <c r="L10" s="16">
-        <v>2</v>
-      </c>
       <c r="M10" s="16">
-        <v>3</v>
-      </c>
-      <c r="N10" s="15">
+        <v>2</v>
+      </c>
+      <c r="N10" s="16">
+        <v>3</v>
+      </c>
+      <c r="O10" s="15">
         <v>9</v>
       </c>
-      <c r="O10" s="16">
-        <v>3</v>
-      </c>
       <c r="P10" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C11" s="15">
         <v>984</v>
       </c>
-      <c r="C11" s="17">
+      <c r="D11" s="17">
         <v>407</v>
       </c>
-      <c r="D11" s="17">
+      <c r="E11" s="17">
         <v>577</v>
       </c>
-      <c r="E11" s="15">
+      <c r="F11" s="15">
         <v>362</v>
       </c>
-      <c r="F11" s="17">
+      <c r="G11" s="17">
         <v>139</v>
       </c>
-      <c r="G11" s="17">
+      <c r="H11" s="17">
         <v>223</v>
       </c>
-      <c r="H11" s="17">
+      <c r="I11" s="17">
         <v>75</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="17">
         <v>12</v>
       </c>
-      <c r="J11" s="17">
+      <c r="K11" s="17">
         <v>63</v>
       </c>
-      <c r="K11" s="17">
+      <c r="L11" s="17">
         <v>287</v>
       </c>
-      <c r="L11" s="17">
+      <c r="M11" s="17">
         <v>127</v>
       </c>
-      <c r="M11" s="17">
+      <c r="N11" s="17">
         <v>160</v>
       </c>
-      <c r="N11" s="15">
+      <c r="O11" s="15">
         <v>622</v>
       </c>
-      <c r="O11" s="17">
+      <c r="P11" s="17">
         <v>268</v>
       </c>
-      <c r="P11" s="17">
+      <c r="Q11" s="17">
         <v>354</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C12" s="15">
         <v>708</v>
       </c>
-      <c r="C12" s="16">
+      <c r="D12" s="16">
         <v>282</v>
       </c>
-      <c r="D12" s="16">
+      <c r="E12" s="16">
         <v>426</v>
       </c>
-      <c r="E12" s="15">
+      <c r="F12" s="15">
         <v>172</v>
       </c>
-      <c r="F12" s="16">
+      <c r="G12" s="16">
         <v>64</v>
       </c>
-      <c r="G12" s="16">
+      <c r="H12" s="16">
         <v>108</v>
       </c>
-      <c r="H12" s="17">
+      <c r="I12" s="17">
         <v>26</v>
       </c>
-      <c r="I12" s="16">
+      <c r="J12" s="16">
         <v>4</v>
       </c>
-      <c r="J12" s="16">
+      <c r="K12" s="16">
         <v>22</v>
       </c>
-      <c r="K12" s="17">
+      <c r="L12" s="17">
         <v>146</v>
       </c>
-      <c r="L12" s="16">
+      <c r="M12" s="16">
         <v>60</v>
       </c>
-      <c r="M12" s="16">
+      <c r="N12" s="16">
         <v>86</v>
       </c>
-      <c r="N12" s="15">
+      <c r="O12" s="15">
         <v>536</v>
       </c>
-      <c r="O12" s="16">
+      <c r="P12" s="16">
         <v>218</v>
       </c>
-      <c r="P12" s="16">
+      <c r="Q12" s="16">
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C13" s="15">
         <v>3979</v>
       </c>
-      <c r="C13" s="17">
+      <c r="D13" s="17">
         <v>1743</v>
       </c>
-      <c r="D13" s="17">
+      <c r="E13" s="17">
         <v>2236</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13" s="15">
         <v>1165</v>
       </c>
-      <c r="F13" s="17">
+      <c r="G13" s="17">
         <v>508</v>
       </c>
-      <c r="G13" s="17">
+      <c r="H13" s="17">
         <v>657</v>
       </c>
-      <c r="H13" s="17">
+      <c r="I13" s="17">
         <v>73</v>
       </c>
-      <c r="I13" s="17">
+      <c r="J13" s="17">
         <v>19</v>
       </c>
-      <c r="J13" s="17">
+      <c r="K13" s="17">
         <v>54</v>
       </c>
-      <c r="K13" s="17">
+      <c r="L13" s="17">
         <v>1092</v>
       </c>
-      <c r="L13" s="17">
+      <c r="M13" s="17">
         <v>489</v>
       </c>
-      <c r="M13" s="17">
+      <c r="N13" s="17">
         <v>603</v>
       </c>
-      <c r="N13" s="15">
+      <c r="O13" s="15">
         <v>2814</v>
       </c>
-      <c r="O13" s="17">
+      <c r="P13" s="17">
         <v>1235</v>
       </c>
-      <c r="P13" s="17">
+      <c r="Q13" s="17">
         <v>1579</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C14" s="15">
         <v>842</v>
       </c>
-      <c r="C14" s="16">
+      <c r="D14" s="16">
         <v>333</v>
       </c>
-      <c r="D14" s="16">
+      <c r="E14" s="16">
         <v>509</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="15">
         <v>263</v>
       </c>
-      <c r="F14" s="16">
+      <c r="G14" s="16">
         <v>94</v>
       </c>
-      <c r="G14" s="16">
+      <c r="H14" s="16">
         <v>169</v>
       </c>
-      <c r="H14" s="17">
+      <c r="I14" s="17">
         <v>54</v>
       </c>
-      <c r="I14" s="16">
-        <v>2</v>
-      </c>
       <c r="J14" s="16">
+        <v>2</v>
+      </c>
+      <c r="K14" s="16">
         <v>52</v>
       </c>
-      <c r="K14" s="17">
+      <c r="L14" s="17">
         <v>209</v>
       </c>
-      <c r="L14" s="16">
+      <c r="M14" s="16">
         <v>92</v>
       </c>
-      <c r="M14" s="16">
+      <c r="N14" s="16">
         <v>117</v>
       </c>
-      <c r="N14" s="15">
+      <c r="O14" s="15">
         <v>579</v>
       </c>
-      <c r="O14" s="16">
+      <c r="P14" s="16">
         <v>239</v>
       </c>
-      <c r="P14" s="16">
+      <c r="Q14" s="16">
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C15" s="15">
         <v>1760</v>
       </c>
-      <c r="C15" s="17">
+      <c r="D15" s="17">
         <v>783</v>
       </c>
-      <c r="D15" s="17">
+      <c r="E15" s="17">
         <v>977</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F15" s="15">
         <v>414</v>
       </c>
-      <c r="F15" s="17">
+      <c r="G15" s="17">
         <v>174</v>
       </c>
-      <c r="G15" s="17">
+      <c r="H15" s="17">
         <v>240</v>
       </c>
-      <c r="H15" s="17">
+      <c r="I15" s="17">
         <v>49</v>
       </c>
-      <c r="I15" s="17">
+      <c r="J15" s="17">
         <v>11</v>
       </c>
-      <c r="J15" s="17">
+      <c r="K15" s="17">
         <v>38</v>
       </c>
-      <c r="K15" s="17">
+      <c r="L15" s="17">
         <v>365</v>
       </c>
-      <c r="L15" s="17">
+      <c r="M15" s="17">
         <v>163</v>
       </c>
-      <c r="M15" s="17">
+      <c r="N15" s="17">
         <v>202</v>
       </c>
-      <c r="N15" s="15">
+      <c r="O15" s="15">
         <v>1346</v>
       </c>
-      <c r="O15" s="17">
+      <c r="P15" s="17">
         <v>609</v>
       </c>
-      <c r="P15" s="17">
+      <c r="Q15" s="17">
         <v>737</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C16" s="15">
         <v>104</v>
       </c>
-      <c r="C16" s="16">
+      <c r="D16" s="16">
         <v>42</v>
       </c>
-      <c r="D16" s="16">
+      <c r="E16" s="16">
         <v>62</v>
       </c>
-      <c r="E16" s="15">
+      <c r="F16" s="15">
         <v>51</v>
       </c>
-      <c r="F16" s="16">
+      <c r="G16" s="16">
         <v>18</v>
       </c>
-      <c r="G16" s="16">
+      <c r="H16" s="16">
         <v>33</v>
       </c>
-      <c r="H16" s="17">
+      <c r="I16" s="17">
         <v>10</v>
       </c>
-      <c r="I16" s="16">
-        <v>1</v>
-      </c>
       <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="16">
         <v>9</v>
       </c>
-      <c r="K16" s="17">
+      <c r="L16" s="17">
         <v>41</v>
       </c>
-      <c r="L16" s="16">
+      <c r="M16" s="16">
         <v>17</v>
       </c>
-      <c r="M16" s="16">
+      <c r="N16" s="16">
         <v>24</v>
       </c>
-      <c r="N16" s="15">
+      <c r="O16" s="15">
         <v>53</v>
       </c>
-      <c r="O16" s="16">
+      <c r="P16" s="16">
         <v>24</v>
       </c>
-      <c r="P16" s="16">
+      <c r="Q16" s="16">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C17" s="15">
         <v>423</v>
       </c>
-      <c r="C17" s="17">
+      <c r="D17" s="17">
         <v>182</v>
       </c>
-      <c r="D17" s="17">
+      <c r="E17" s="17">
         <v>241</v>
       </c>
-      <c r="E17" s="15">
+      <c r="F17" s="15">
         <v>192</v>
       </c>
-      <c r="F17" s="17">
+      <c r="G17" s="17">
         <v>74</v>
       </c>
-      <c r="G17" s="17">
+      <c r="H17" s="17">
         <v>118</v>
       </c>
-      <c r="H17" s="17">
+      <c r="I17" s="17">
         <v>61</v>
       </c>
-      <c r="I17" s="17">
+      <c r="J17" s="17">
         <v>11</v>
       </c>
-      <c r="J17" s="17">
+      <c r="K17" s="17">
         <v>50</v>
       </c>
-      <c r="K17" s="17">
+      <c r="L17" s="17">
         <v>131</v>
       </c>
-      <c r="L17" s="17">
+      <c r="M17" s="17">
         <v>63</v>
       </c>
-      <c r="M17" s="17">
+      <c r="N17" s="17">
         <v>68</v>
       </c>
-      <c r="N17" s="15">
+      <c r="O17" s="15">
         <v>231</v>
       </c>
-      <c r="O17" s="17">
+      <c r="P17" s="17">
         <v>108</v>
       </c>
-      <c r="P17" s="17">
+      <c r="Q17" s="17">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C18" s="15">
         <v>165</v>
       </c>
-      <c r="C18" s="16">
+      <c r="D18" s="16">
         <v>70</v>
       </c>
-      <c r="D18" s="16">
+      <c r="E18" s="16">
         <v>95</v>
       </c>
-      <c r="E18" s="15">
+      <c r="F18" s="15">
         <v>86</v>
       </c>
-      <c r="F18" s="16">
+      <c r="G18" s="16">
         <v>30</v>
       </c>
-      <c r="G18" s="16">
+      <c r="H18" s="16">
         <v>56</v>
       </c>
-      <c r="H18" s="17">
+      <c r="I18" s="17">
         <v>4</v>
       </c>
-      <c r="I18" s="16">
-        <v>0</v>
-      </c>
       <c r="J18" s="16">
+        <v>0</v>
+      </c>
+      <c r="K18" s="16">
         <v>4</v>
       </c>
-      <c r="K18" s="17">
+      <c r="L18" s="17">
         <v>82</v>
       </c>
-      <c r="L18" s="16">
+      <c r="M18" s="16">
         <v>30</v>
       </c>
-      <c r="M18" s="16">
+      <c r="N18" s="16">
         <v>52</v>
       </c>
-      <c r="N18" s="15">
+      <c r="O18" s="15">
         <v>79</v>
       </c>
-      <c r="O18" s="16">
+      <c r="P18" s="16">
         <v>40</v>
       </c>
-      <c r="P18" s="16">
+      <c r="Q18" s="16">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C19" s="15">
         <v>1487</v>
       </c>
-      <c r="C19" s="17">
+      <c r="D19" s="17">
         <v>626</v>
       </c>
-      <c r="D19" s="17">
+      <c r="E19" s="17">
         <v>861</v>
       </c>
-      <c r="E19" s="15">
+      <c r="F19" s="15">
         <v>414</v>
       </c>
-      <c r="F19" s="17">
+      <c r="G19" s="17">
         <v>167</v>
       </c>
-      <c r="G19" s="17">
+      <c r="H19" s="17">
         <v>247</v>
       </c>
-      <c r="H19" s="17">
+      <c r="I19" s="17">
         <v>74</v>
       </c>
-      <c r="I19" s="17">
+      <c r="J19" s="17">
         <v>10</v>
       </c>
-      <c r="J19" s="17">
+      <c r="K19" s="17">
         <v>64</v>
       </c>
-      <c r="K19" s="17">
+      <c r="L19" s="17">
         <v>340</v>
       </c>
-      <c r="L19" s="17">
+      <c r="M19" s="17">
         <v>157</v>
       </c>
-      <c r="M19" s="17">
+      <c r="N19" s="17">
         <v>183</v>
       </c>
-      <c r="N19" s="15">
+      <c r="O19" s="15">
         <v>1073</v>
       </c>
-      <c r="O19" s="17">
+      <c r="P19" s="17">
         <v>459</v>
       </c>
-      <c r="P19" s="17">
+      <c r="Q19" s="17">
         <v>614</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C20" s="15">
         <v>606</v>
       </c>
-      <c r="C20" s="16">
+      <c r="D20" s="16">
         <v>262</v>
       </c>
-      <c r="D20" s="16">
+      <c r="E20" s="16">
         <v>344</v>
       </c>
-      <c r="E20" s="15">
+      <c r="F20" s="15">
         <v>164</v>
       </c>
-      <c r="F20" s="16">
+      <c r="G20" s="16">
         <v>72</v>
       </c>
-      <c r="G20" s="16">
+      <c r="H20" s="16">
         <v>92</v>
       </c>
-      <c r="H20" s="17">
+      <c r="I20" s="17">
         <v>20</v>
       </c>
-      <c r="I20" s="16">
+      <c r="J20" s="16">
         <v>6</v>
       </c>
-      <c r="J20" s="16">
+      <c r="K20" s="16">
         <v>14</v>
       </c>
-      <c r="K20" s="17">
+      <c r="L20" s="17">
         <v>144</v>
       </c>
-      <c r="L20" s="16">
+      <c r="M20" s="16">
         <v>66</v>
       </c>
-      <c r="M20" s="16">
+      <c r="N20" s="16">
         <v>78</v>
       </c>
-      <c r="N20" s="15">
+      <c r="O20" s="15">
         <v>442</v>
       </c>
-      <c r="O20" s="16">
+      <c r="P20" s="16">
         <v>190</v>
       </c>
-      <c r="P20" s="16">
+      <c r="Q20" s="16">
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C21" s="15">
         <v>129</v>
       </c>
-      <c r="C21" s="17">
+      <c r="D21" s="17">
         <v>53</v>
       </c>
-      <c r="D21" s="17">
+      <c r="E21" s="17">
         <v>76</v>
       </c>
-      <c r="E21" s="15">
+      <c r="F21" s="15">
         <v>52</v>
       </c>
-      <c r="F21" s="17">
+      <c r="G21" s="17">
         <v>21</v>
       </c>
-      <c r="G21" s="17">
+      <c r="H21" s="17">
         <v>31</v>
       </c>
-      <c r="H21" s="17">
+      <c r="I21" s="17">
         <v>6</v>
       </c>
-      <c r="I21" s="17">
-        <v>0</v>
-      </c>
       <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
         <v>6</v>
       </c>
-      <c r="K21" s="17">
+      <c r="L21" s="17">
         <v>46</v>
       </c>
-      <c r="L21" s="17">
+      <c r="M21" s="17">
         <v>21</v>
       </c>
-      <c r="M21" s="17">
+      <c r="N21" s="17">
         <v>25</v>
       </c>
-      <c r="N21" s="15">
+      <c r="O21" s="15">
         <v>77</v>
       </c>
-      <c r="O21" s="17">
+      <c r="P21" s="17">
         <v>32</v>
       </c>
-      <c r="P21" s="17">
+      <c r="Q21" s="17">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C22" s="15">
         <v>101</v>
       </c>
-      <c r="C22" s="16">
+      <c r="D22" s="16">
         <v>43</v>
       </c>
-      <c r="D22" s="16">
+      <c r="E22" s="16">
         <v>58</v>
       </c>
-      <c r="E22" s="15">
+      <c r="F22" s="15">
         <v>36</v>
       </c>
-      <c r="F22" s="16">
+      <c r="G22" s="16">
         <v>14</v>
       </c>
-      <c r="G22" s="16">
+      <c r="H22" s="16">
         <v>22</v>
       </c>
-      <c r="H22" s="17">
-        <v>3</v>
-      </c>
-      <c r="I22" s="16">
-        <v>1</v>
+      <c r="I22" s="17">
+        <v>3</v>
       </c>
       <c r="J22" s="16">
-        <v>2</v>
-      </c>
-      <c r="K22" s="17">
+        <v>1</v>
+      </c>
+      <c r="K22" s="16">
+        <v>2</v>
+      </c>
+      <c r="L22" s="17">
         <v>33</v>
       </c>
-      <c r="L22" s="16">
+      <c r="M22" s="16">
         <v>13</v>
       </c>
-      <c r="M22" s="16">
+      <c r="N22" s="16">
         <v>20</v>
       </c>
-      <c r="N22" s="15">
+      <c r="O22" s="15">
         <v>65</v>
       </c>
-      <c r="O22" s="16">
+      <c r="P22" s="16">
         <v>29</v>
       </c>
-      <c r="P22" s="16">
+      <c r="Q22" s="16">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C23" s="15">
         <v>308</v>
       </c>
-      <c r="C23" s="17">
+      <c r="D23" s="17">
         <v>138</v>
       </c>
-      <c r="D23" s="17">
+      <c r="E23" s="17">
         <v>170</v>
       </c>
-      <c r="E23" s="15">
+      <c r="F23" s="15">
         <v>85</v>
       </c>
-      <c r="F23" s="17">
+      <c r="G23" s="17">
         <v>41</v>
       </c>
-      <c r="G23" s="17">
+      <c r="H23" s="17">
         <v>44</v>
       </c>
-      <c r="H23" s="17">
+      <c r="I23" s="17">
         <v>14</v>
       </c>
-      <c r="I23" s="17">
+      <c r="J23" s="17">
         <v>4</v>
       </c>
-      <c r="J23" s="17">
+      <c r="K23" s="17">
         <v>10</v>
       </c>
-      <c r="K23" s="17">
+      <c r="L23" s="17">
         <v>71</v>
       </c>
-      <c r="L23" s="17">
+      <c r="M23" s="17">
         <v>37</v>
       </c>
-      <c r="M23" s="17">
+      <c r="N23" s="17">
         <v>34</v>
       </c>
-      <c r="N23" s="15">
+      <c r="O23" s="15">
         <v>223</v>
       </c>
-      <c r="O23" s="17">
+      <c r="P23" s="17">
         <v>97</v>
       </c>
-      <c r="P23" s="17">
+      <c r="Q23" s="17">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C24" s="15">
         <v>474</v>
       </c>
-      <c r="C24" s="16">
+      <c r="D24" s="16">
         <v>220</v>
       </c>
-      <c r="D24" s="16">
+      <c r="E24" s="16">
         <v>254</v>
       </c>
-      <c r="E24" s="15">
+      <c r="F24" s="15">
         <v>167</v>
       </c>
-      <c r="F24" s="16">
+      <c r="G24" s="16">
         <v>69</v>
       </c>
-      <c r="G24" s="16">
+      <c r="H24" s="16">
         <v>98</v>
       </c>
-      <c r="H24" s="17">
+      <c r="I24" s="17">
         <v>37</v>
       </c>
-      <c r="I24" s="16">
-        <v>3</v>
-      </c>
       <c r="J24" s="16">
+        <v>3</v>
+      </c>
+      <c r="K24" s="16">
         <v>34</v>
       </c>
-      <c r="K24" s="17">
+      <c r="L24" s="17">
         <v>130</v>
       </c>
-      <c r="L24" s="16">
+      <c r="M24" s="16">
         <v>66</v>
       </c>
-      <c r="M24" s="16">
+      <c r="N24" s="16">
         <v>64</v>
       </c>
-      <c r="N24" s="15">
+      <c r="O24" s="15">
         <v>307</v>
       </c>
-      <c r="O24" s="16">
+      <c r="P24" s="16">
         <v>151</v>
       </c>
-      <c r="P24" s="16">
+      <c r="Q24" s="16">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C25" s="15">
         <v>1046</v>
       </c>
-      <c r="C25" s="17">
+      <c r="D25" s="17">
         <v>438</v>
       </c>
-      <c r="D25" s="17">
+      <c r="E25" s="17">
         <v>608</v>
       </c>
-      <c r="E25" s="15">
+      <c r="F25" s="15">
         <v>307</v>
       </c>
-      <c r="F25" s="17">
+      <c r="G25" s="17">
         <v>120</v>
       </c>
-      <c r="G25" s="17">
+      <c r="H25" s="17">
         <v>187</v>
       </c>
-      <c r="H25" s="17">
+      <c r="I25" s="17">
         <v>37</v>
       </c>
-      <c r="I25" s="17">
+      <c r="J25" s="17">
         <v>4</v>
       </c>
-      <c r="J25" s="17">
+      <c r="K25" s="17">
         <v>33</v>
       </c>
-      <c r="K25" s="17">
+      <c r="L25" s="17">
         <v>270</v>
       </c>
-      <c r="L25" s="17">
+      <c r="M25" s="17">
         <v>116</v>
       </c>
-      <c r="M25" s="17">
+      <c r="N25" s="17">
         <v>154</v>
       </c>
-      <c r="N25" s="15">
+      <c r="O25" s="15">
         <v>739</v>
       </c>
-      <c r="O25" s="17">
+      <c r="P25" s="17">
         <v>318</v>
       </c>
-      <c r="P25" s="17">
+      <c r="Q25" s="17">
         <v>421</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C26" s="15">
         <v>1666</v>
       </c>
-      <c r="C26" s="16">
+      <c r="D26" s="16">
         <v>717</v>
       </c>
-      <c r="D26" s="16">
+      <c r="E26" s="16">
         <v>949</v>
       </c>
-      <c r="E26" s="15">
+      <c r="F26" s="15">
         <v>490</v>
       </c>
-      <c r="F26" s="16">
+      <c r="G26" s="16">
         <v>181</v>
       </c>
-      <c r="G26" s="16">
+      <c r="H26" s="16">
         <v>309</v>
       </c>
-      <c r="H26" s="17">
+      <c r="I26" s="17">
         <v>82</v>
       </c>
-      <c r="I26" s="16">
+      <c r="J26" s="16">
         <v>9</v>
       </c>
-      <c r="J26" s="16">
+      <c r="K26" s="16">
         <v>73</v>
       </c>
-      <c r="K26" s="17">
+      <c r="L26" s="17">
         <v>408</v>
       </c>
-      <c r="L26" s="16">
+      <c r="M26" s="16">
         <v>172</v>
       </c>
-      <c r="M26" s="16">
+      <c r="N26" s="16">
         <v>236</v>
       </c>
-      <c r="N26" s="15">
+      <c r="O26" s="15">
         <v>1176</v>
       </c>
-      <c r="O26" s="16">
+      <c r="P26" s="16">
         <v>536</v>
       </c>
-      <c r="P26" s="16">
+      <c r="Q26" s="16">
         <v>640</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C27" s="15">
         <v>327</v>
       </c>
-      <c r="C27" s="17">
+      <c r="D27" s="17">
         <v>130</v>
       </c>
-      <c r="D27" s="17">
+      <c r="E27" s="17">
         <v>197</v>
       </c>
-      <c r="E27" s="15">
+      <c r="F27" s="15">
         <v>104</v>
       </c>
-      <c r="F27" s="17">
+      <c r="G27" s="17">
         <v>33</v>
       </c>
-      <c r="G27" s="17">
+      <c r="H27" s="17">
         <v>71</v>
       </c>
-      <c r="H27" s="17">
+      <c r="I27" s="17">
         <v>21</v>
       </c>
-      <c r="I27" s="17">
-        <v>2</v>
-      </c>
       <c r="J27" s="17">
+        <v>2</v>
+      </c>
+      <c r="K27" s="17">
         <v>19</v>
       </c>
-      <c r="K27" s="17">
+      <c r="L27" s="17">
         <v>83</v>
       </c>
-      <c r="L27" s="17">
+      <c r="M27" s="17">
         <v>31</v>
       </c>
-      <c r="M27" s="17">
+      <c r="N27" s="17">
         <v>52</v>
       </c>
-      <c r="N27" s="15">
+      <c r="O27" s="15">
         <v>223</v>
       </c>
-      <c r="O27" s="17">
+      <c r="P27" s="17">
         <v>97</v>
       </c>
-      <c r="P27" s="17">
+      <c r="Q27" s="17">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C28" s="15">
         <v>573</v>
       </c>
-      <c r="C28" s="16">
+      <c r="D28" s="16">
         <v>249</v>
       </c>
-      <c r="D28" s="16">
+      <c r="E28" s="16">
         <v>324</v>
       </c>
-      <c r="E28" s="15">
+      <c r="F28" s="15">
         <v>76</v>
       </c>
-      <c r="F28" s="16">
+      <c r="G28" s="16">
         <v>30</v>
       </c>
-      <c r="G28" s="16">
+      <c r="H28" s="16">
         <v>46</v>
       </c>
-      <c r="H28" s="17">
+      <c r="I28" s="17">
         <v>9</v>
       </c>
-      <c r="I28" s="16">
-        <v>2</v>
-      </c>
       <c r="J28" s="16">
+        <v>2</v>
+      </c>
+      <c r="K28" s="16">
         <v>7</v>
       </c>
-      <c r="K28" s="17">
+      <c r="L28" s="17">
         <v>67</v>
       </c>
-      <c r="L28" s="16">
+      <c r="M28" s="16">
         <v>28</v>
       </c>
-      <c r="M28" s="16">
+      <c r="N28" s="16">
         <v>39</v>
       </c>
-      <c r="N28" s="15">
+      <c r="O28" s="15">
         <v>497</v>
       </c>
-      <c r="O28" s="16">
+      <c r="P28" s="16">
         <v>219</v>
       </c>
-      <c r="P28" s="16">
+      <c r="Q28" s="16">
         <v>278</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C29" s="15">
         <v>69</v>
       </c>
-      <c r="C29" s="17">
+      <c r="D29" s="17">
         <v>33</v>
       </c>
-      <c r="D29" s="17">
+      <c r="E29" s="17">
         <v>36</v>
       </c>
-      <c r="E29" s="15">
+      <c r="F29" s="15">
         <v>37</v>
       </c>
-      <c r="F29" s="17">
+      <c r="G29" s="17">
         <v>14</v>
       </c>
-      <c r="G29" s="17">
+      <c r="H29" s="17">
         <v>23</v>
       </c>
-      <c r="H29" s="17">
+      <c r="I29" s="17">
         <v>5</v>
       </c>
-      <c r="I29" s="17">
-        <v>1</v>
-      </c>
       <c r="J29" s="17">
+        <v>1</v>
+      </c>
+      <c r="K29" s="17">
         <v>4</v>
       </c>
-      <c r="K29" s="17">
+      <c r="L29" s="17">
         <v>32</v>
       </c>
-      <c r="L29" s="17">
+      <c r="M29" s="17">
         <v>13</v>
       </c>
-      <c r="M29" s="17">
+      <c r="N29" s="17">
         <v>19</v>
       </c>
-      <c r="N29" s="15">
+      <c r="O29" s="15">
         <v>32</v>
       </c>
-      <c r="O29" s="17">
+      <c r="P29" s="17">
         <v>19</v>
       </c>
-      <c r="P29" s="17">
+      <c r="Q29" s="17">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C30" s="15">
         <v>2250</v>
       </c>
-      <c r="C30" s="16">
+      <c r="D30" s="16">
         <v>1020</v>
       </c>
-      <c r="D30" s="16">
+      <c r="E30" s="16">
         <v>1230</v>
       </c>
-      <c r="E30" s="15">
+      <c r="F30" s="15">
         <v>519</v>
       </c>
-      <c r="F30" s="16">
+      <c r="G30" s="16">
         <v>228</v>
       </c>
-      <c r="G30" s="16">
+      <c r="H30" s="16">
         <v>291</v>
       </c>
-      <c r="H30" s="17">
+      <c r="I30" s="17">
         <v>39</v>
       </c>
-      <c r="I30" s="16">
+      <c r="J30" s="16">
         <v>9</v>
       </c>
-      <c r="J30" s="16">
+      <c r="K30" s="16">
         <v>30</v>
       </c>
-      <c r="K30" s="17">
+      <c r="L30" s="17">
         <v>480</v>
       </c>
-      <c r="L30" s="16">
+      <c r="M30" s="16">
         <v>219</v>
       </c>
-      <c r="M30" s="16">
+      <c r="N30" s="16">
         <v>261</v>
       </c>
-      <c r="N30" s="15">
+      <c r="O30" s="15">
         <v>1731</v>
       </c>
-      <c r="O30" s="16">
+      <c r="P30" s="16">
         <v>792</v>
       </c>
-      <c r="P30" s="16">
+      <c r="Q30" s="16">
         <v>939</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C31" s="15">
         <v>700</v>
       </c>
-      <c r="C31" s="17">
+      <c r="D31" s="17">
         <v>290</v>
       </c>
-      <c r="D31" s="17">
+      <c r="E31" s="17">
         <v>410</v>
       </c>
-      <c r="E31" s="15">
+      <c r="F31" s="15">
         <v>240</v>
       </c>
-      <c r="F31" s="17">
+      <c r="G31" s="17">
         <v>86</v>
       </c>
-      <c r="G31" s="17">
+      <c r="H31" s="17">
         <v>154</v>
       </c>
-      <c r="H31" s="17">
+      <c r="I31" s="17">
         <v>51</v>
       </c>
-      <c r="I31" s="17">
+      <c r="J31" s="17">
         <v>4</v>
       </c>
-      <c r="J31" s="17">
+      <c r="K31" s="17">
         <v>47</v>
       </c>
-      <c r="K31" s="17">
+      <c r="L31" s="17">
         <v>189</v>
       </c>
-      <c r="L31" s="17">
+      <c r="M31" s="17">
         <v>82</v>
       </c>
-      <c r="M31" s="17">
+      <c r="N31" s="17">
         <v>107</v>
       </c>
-      <c r="N31" s="15">
+      <c r="O31" s="15">
         <v>460</v>
       </c>
-      <c r="O31" s="17">
+      <c r="P31" s="17">
         <v>204</v>
       </c>
-      <c r="P31" s="17">
+      <c r="Q31" s="17">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C32" s="15">
         <v>326</v>
       </c>
-      <c r="C32" s="16">
+      <c r="D32" s="16">
         <v>130</v>
       </c>
-      <c r="D32" s="16">
+      <c r="E32" s="16">
         <v>196</v>
       </c>
-      <c r="E32" s="15">
+      <c r="F32" s="15">
         <v>103</v>
       </c>
-      <c r="F32" s="16">
+      <c r="G32" s="16">
         <v>44</v>
       </c>
-      <c r="G32" s="16">
+      <c r="H32" s="16">
         <v>59</v>
       </c>
-      <c r="H32" s="17">
+      <c r="I32" s="17">
         <v>18</v>
       </c>
-      <c r="I32" s="16">
-        <v>2</v>
-      </c>
       <c r="J32" s="16">
+        <v>2</v>
+      </c>
+      <c r="K32" s="16">
         <v>16</v>
       </c>
-      <c r="K32" s="17">
+      <c r="L32" s="17">
         <v>85</v>
       </c>
-      <c r="L32" s="16">
+      <c r="M32" s="16">
         <v>42</v>
       </c>
-      <c r="M32" s="16">
+      <c r="N32" s="16">
         <v>43</v>
       </c>
-      <c r="N32" s="15">
+      <c r="O32" s="15">
         <v>223</v>
       </c>
-      <c r="O32" s="16">
+      <c r="P32" s="16">
         <v>86</v>
       </c>
-      <c r="P32" s="16">
+      <c r="Q32" s="16">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="30">
+      <c r="B33" s="82">
+        <v>2010</v>
+      </c>
+      <c r="C33" s="30">
         <v>4345</v>
       </c>
-      <c r="C33" s="31">
+      <c r="D33" s="31">
         <v>1768</v>
       </c>
-      <c r="D33" s="31">
+      <c r="E33" s="31">
         <v>2577</v>
       </c>
-      <c r="E33" s="30">
+      <c r="F33" s="30">
         <v>1312</v>
       </c>
-      <c r="F33" s="31">
+      <c r="G33" s="31">
         <v>486</v>
       </c>
-      <c r="G33" s="31">
+      <c r="H33" s="31">
         <v>826</v>
       </c>
-      <c r="H33" s="31">
+      <c r="I33" s="31">
         <v>151</v>
       </c>
-      <c r="I33" s="31">
+      <c r="J33" s="31">
         <v>31</v>
       </c>
-      <c r="J33" s="31">
+      <c r="K33" s="31">
         <v>120</v>
       </c>
-      <c r="K33" s="31">
+      <c r="L33" s="31">
         <v>1161</v>
       </c>
-      <c r="L33" s="31">
+      <c r="M33" s="31">
         <v>455</v>
       </c>
-      <c r="M33" s="31">
+      <c r="N33" s="31">
         <v>706</v>
       </c>
-      <c r="N33" s="30">
+      <c r="O33" s="30">
         <v>3033</v>
       </c>
-      <c r="O33" s="31">
+      <c r="P33" s="31">
         <v>1282</v>
       </c>
-      <c r="P33" s="31">
+      <c r="Q33" s="31">
         <v>1751</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.51181102362204722" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -61022,7 +61124,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>